<commit_message>
modif cellule A1 en vide
</commit_message>
<xml_diff>
--- a/feuille.xlsx
+++ b/feuille.xlsx
@@ -21,10 +21,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Cellule A1</t>
+    <t>Cellule A2</t>
   </si>
   <si>
-    <t>Cellule A2</t>
+    <t>Cellule A1 vide</t>
   </si>
 </sst>
 </file>
@@ -345,19 +345,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
colorier en jaune la colonne B
</commit_message>
<xml_diff>
--- a/feuille.xlsx
+++ b/feuille.xlsx
@@ -46,12 +46,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +72,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,13 +355,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>